<commit_message>
excel read and write file
</commit_message>
<xml_diff>
--- a/ExcelUtils/testData.xlsx
+++ b/ExcelUtils/testData.xlsx
@@ -1,31 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\61491\ExcelUtils\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B082E9E-2687-46F4-9604-FAE7FDBAB778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Sno</t>
   </si>
@@ -45,53 +34,56 @@
     <t>Mango</t>
   </si>
   <si>
-    <t>Apple</t>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>350</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>Iphone</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Winter</t>
   </si>
   <si>
     <t>Papaya</t>
   </si>
   <si>
-    <t>Banana</t>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>Replace text</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
   <si>
     <t>Kiwi</t>
   </si>
   <si>
-    <t>Orange</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Yellow</t>
-  </si>
-  <si>
     <t>Green</t>
-  </si>
-  <si>
-    <t>Summer</t>
-  </si>
-  <si>
-    <t>Winter</t>
-  </si>
-  <si>
-    <t>Spring</t>
-  </si>
-  <si>
-    <t>All</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -398,20 +390,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="13.36328125" customWidth="1"/>
     <col min="3" max="3" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -428,7 +420,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -436,98 +428,98 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1">
-        <v>299</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1">
         <v>345</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1">
         <v>187</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1">
         <v>69</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1">
         <v>399</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1">
         <v>199</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>